<commit_message>
yellow marked rows deleted
</commit_message>
<xml_diff>
--- a/budgetportal/tests/test_data/test_import_prov_infra_projects.xlsx
+++ b/budgetportal/tests/test_data/test_import_prov_infra_projects.xlsx
@@ -383,7 +383,7 @@
     <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="167" formatCode="\ * #,##0.00\ ;\-* #,##0.00\ ;\ * \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -406,95 +406,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -502,63 +413,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -566,23 +429,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,59 +456,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -673,100 +470,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Accent 1 17" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 16" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2 18" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3 19" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad 13" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error 15" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote 8" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good 11" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1 4" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2 5" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 3" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink 9" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral 12" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note 7" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status 10" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text 6" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning 14" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -775,10 +491,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CR51"/>
+  <dimension ref="A1:CR12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="AB13" activeCellId="0" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2223,108 +1939,6 @@
       <c r="AV12" s="0" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB26" s="4"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB27" s="4"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB28" s="4"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB32" s="4"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB33" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB48" s="4"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB50" s="4"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB51" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
WIP cleaning up config and docs
</commit_message>
<xml_diff>
--- a/budgetportal/tests/test_data/test_import_prov_infra_projects.xlsx
+++ b/budgetportal/tests/test_data/test_import_prov_infra_projects.xlsx
@@ -283,7 +283,7 @@
     <t xml:space="preserve">Principal Agent:  </t>
   </si>
   <si>
-    <t xml:space="preserve">Principal Agent:  Nelson Barabosa Architects</t>
+    <t xml:space="preserve">Principal Agent:  This them that</t>
   </si>
   <si>
     <t xml:space="preserve">Modded Modular Library</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">Pre - Feasibility</t>
   </si>
   <si>
-    <t xml:space="preserve">Principal Agent:  Fabricated Steel Manufacturing</t>
+    <t xml:space="preserve">Principal Agent:  Fred’s Steel Manufacturing</t>
   </si>
   <si>
     <t xml:space="preserve">Dreizehn Laerskool</t>
@@ -463,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:CH12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP1" activeCellId="0" sqref="AP1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,7 +755,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>-30.03029</v>
+        <v>-30.13029</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>29.60355</v>
@@ -850,7 +850,7 @@
         <v>53</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>-29.96148</v>
+        <v>-29.86148</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>30.21308</v>
@@ -948,7 +948,7 @@
         <v>58</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>-30.0057</v>
+        <v>-30.1057</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>30.92655</v>
@@ -1040,7 +1040,7 @@
         <v>53</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>-29.64888</v>
+        <v>-29.54888</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>30.39356</v>
@@ -1254,7 +1254,7 @@
         <v>75</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>-32.33235</v>
+        <v>-32.23235</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>28.14463</v>
@@ -1364,7 +1364,7 @@
         <v>83</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>-31.1595994</v>
+        <v>-31.0595994</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>28.8946309</v>
@@ -1457,7 +1457,7 @@
         <v>90</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>-31.6727543</v>
+        <v>-31.5727543</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>27.9834738</v>
@@ -1552,7 +1552,7 @@
         <v>97</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>-26.8472</v>
+        <v>-24.8472</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>26.76787</v>
@@ -1647,7 +1647,7 @@
         <v>75</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>-32.76633</v>
+        <v>-32.66633</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>26.61996</v>
@@ -1739,7 +1739,7 @@
         <v>97</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>-26.84655</v>
+        <v>-26.74655</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>26.86567</v>

</xml_diff>